<commit_message>
Wrote some of chapter 3, output kable still not scrollable
</commit_message>
<xml_diff>
--- a/data/nyts-codebook.xlsx
+++ b/data/nyts-codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StudyResources\Columbia\STATW5702\Final Project\youth-smoking-edav\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C29BA38-4E57-46CA-BA18-EED69FB7D054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B1026-8BB5-4B41-9973-B6B752088269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{E70BE8B0-59DF-4698-B172-61E23C34608B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
   <si>
     <t>Year</t>
   </si>
@@ -84,12 +84,6 @@
     <t>If one of your best friends were to offer you a cigarette, would you smoke it?</t>
   </si>
   <si>
-    <t>Have you ever been curious about smoking a cigar, cigarillo, or little cigar?</t>
-  </si>
-  <si>
-    <t>Have you ever been curious about using chewing tobacco, snuff, or dip?</t>
-  </si>
-  <si>
     <t>Have you ever been curious about using an e-cigarette?</t>
   </si>
   <si>
@@ -141,15 +135,9 @@
     <t>QN34</t>
   </si>
   <si>
-    <t>QN40</t>
-  </si>
-  <si>
     <t>QN35</t>
   </si>
   <si>
-    <t>QN47</t>
-  </si>
-  <si>
     <t>QN44</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
     <t>Q18</t>
   </si>
   <si>
-    <t>Q30</t>
-  </si>
-  <si>
     <t>Q27</t>
   </si>
   <si>
@@ -325,6 +310,30 @@
   </si>
   <si>
     <t>Q5E</t>
+  </si>
+  <si>
+    <t>How old were you when you first smoked a cigar, cigarillo, or little cigar, even one or two puffs?</t>
+  </si>
+  <si>
+    <t>How old were you when you first used chewing tobacco, snuff, or dip, even just a small amount?</t>
+  </si>
+  <si>
+    <t>QN36</t>
+  </si>
+  <si>
+    <t>QN45</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>Q26</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,34 +734,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
@@ -791,22 +800,22 @@
         <v>15</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -814,97 +823,97 @@
         <v>2020</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -912,97 +921,97 @@
         <v>2019</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1010,168 +1019,294 @@
         <v>2018</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="S4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="V4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="AE4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Factor codes in preprocessing
</commit_message>
<xml_diff>
--- a/data/nyts-codebook.xlsx
+++ b/data/nyts-codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StudyResources\Columbia\STATW5702\Final Project\youth-smoking-edav\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B1026-8BB5-4B41-9973-B6B752088269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AF75D6-28A8-449F-92FA-D53DAB768567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{E70BE8B0-59DF-4698-B172-61E23C34608B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="144">
   <si>
     <t>Year</t>
   </si>
@@ -147,75 +147,6 @@
     <t>QN6</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>Q8</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
-    <t>Q10</t>
-  </si>
-  <si>
-    <t>Q11</t>
-  </si>
-  <si>
-    <t>Q12</t>
-  </si>
-  <si>
-    <t>Q13</t>
-  </si>
-  <si>
-    <t>Q14</t>
-  </si>
-  <si>
-    <t>Q15</t>
-  </si>
-  <si>
-    <t>Q16</t>
-  </si>
-  <si>
-    <t>Q17</t>
-  </si>
-  <si>
-    <t>Q23</t>
-  </si>
-  <si>
-    <t>Q18</t>
-  </si>
-  <si>
-    <t>Q27</t>
-  </si>
-  <si>
-    <t>Q43</t>
-  </si>
-  <si>
-    <t>Q34</t>
-  </si>
-  <si>
-    <t>Q19</t>
-  </si>
-  <si>
-    <t>Q24</t>
-  </si>
-  <si>
-    <t>Q28</t>
-  </si>
-  <si>
     <t>Have you ever smoked a cigar, cigarillo, or little cigar, even one or two puffs?</t>
   </si>
   <si>
@@ -282,36 +213,6 @@
     <t>QN5E</t>
   </si>
   <si>
-    <t>Q4A</t>
-  </si>
-  <si>
-    <t>Q4B</t>
-  </si>
-  <si>
-    <t>Q4C</t>
-  </si>
-  <si>
-    <t>Q4D</t>
-  </si>
-  <si>
-    <t>Q4E</t>
-  </si>
-  <si>
-    <t>Q5A</t>
-  </si>
-  <si>
-    <t>Q5B</t>
-  </si>
-  <si>
-    <t>Q5C</t>
-  </si>
-  <si>
-    <t>Q5D</t>
-  </si>
-  <si>
-    <t>Q5E</t>
-  </si>
-  <si>
     <t>How old were you when you first smoked a cigar, cigarillo, or little cigar, even one or two puffs?</t>
   </si>
   <si>
@@ -324,16 +225,247 @@
     <t>QN45</t>
   </si>
   <si>
-    <t>Q20</t>
-  </si>
-  <si>
-    <t>Q25</t>
-  </si>
-  <si>
-    <t>Q22</t>
-  </si>
-  <si>
-    <t>Q26</t>
+    <t>When you are using the Internet, how often do you see ads or promotions for cigarettes or other tobacco products?</t>
+  </si>
+  <si>
+    <t>When you go to a convenience store, supermarket, or gas station, how often do you see ads or promotions for cigarettes or other tobacco products?</t>
+  </si>
+  <si>
+    <t>When you watch TV or streaming services (such as Netflix, Hulu, or Amazon Prime), or go to the movies, how often do you see ads or promotions for cigarettes or other tobacco products?</t>
+  </si>
+  <si>
+    <t>When you are using the Internet, how often do you see ads or promotions for e-cigarettes?</t>
+  </si>
+  <si>
+    <t>When you go to a convenience store, supermarket, or gas station, how often do you see ads or promotions for e-cigarettes?</t>
+  </si>
+  <si>
+    <t>When you watch TV or streaming services (such as Netflix, Hulu, or Amazon Prime), or go to the movies, how often do you see ads or promotions for e-cigarettes?</t>
+  </si>
+  <si>
+    <t>How often do you see posts related to e-cigarettes when you go on social media (such as YouTube, Instagram, Snapchat, Twitter, or Facebook)?</t>
+  </si>
+  <si>
+    <t>QN98</t>
+  </si>
+  <si>
+    <t>QN100</t>
+  </si>
+  <si>
+    <t>QN101</t>
+  </si>
+  <si>
+    <t>QN102</t>
+  </si>
+  <si>
+    <t>QN104</t>
+  </si>
+  <si>
+    <t>QN105</t>
+  </si>
+  <si>
+    <t>QN106</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>QN7</t>
+  </si>
+  <si>
+    <t>QN8</t>
+  </si>
+  <si>
+    <t>QN9</t>
+  </si>
+  <si>
+    <t>QN10</t>
+  </si>
+  <si>
+    <t>QN11</t>
+  </si>
+  <si>
+    <t>QN12</t>
+  </si>
+  <si>
+    <t>QN13</t>
+  </si>
+  <si>
+    <t>QN14</t>
+  </si>
+  <si>
+    <t>QN15</t>
+  </si>
+  <si>
+    <t>QN16</t>
+  </si>
+  <si>
+    <t>QN18</t>
+  </si>
+  <si>
+    <t>QN19</t>
+  </si>
+  <si>
+    <t>QN28</t>
+  </si>
+  <si>
+    <t>QN43</t>
+  </si>
+  <si>
+    <t>QN89</t>
+  </si>
+  <si>
+    <t>QN91</t>
+  </si>
+  <si>
+    <t>QN92</t>
+  </si>
+  <si>
+    <t>QN93</t>
+  </si>
+  <si>
+    <t>QN95</t>
+  </si>
+  <si>
+    <t>QN96</t>
+  </si>
+  <si>
+    <t>How old were you when you first used an e-cigarette, even once or twice?</t>
+  </si>
+  <si>
+    <t>Qn1</t>
+  </si>
+  <si>
+    <t>Qn2</t>
+  </si>
+  <si>
+    <t>Qn3</t>
+  </si>
+  <si>
+    <t>Qn7</t>
+  </si>
+  <si>
+    <t>Qn8</t>
+  </si>
+  <si>
+    <t>Qn9</t>
+  </si>
+  <si>
+    <t>Qn11</t>
+  </si>
+  <si>
+    <t>Qn10</t>
+  </si>
+  <si>
+    <t>Qn12</t>
+  </si>
+  <si>
+    <t>Qn13</t>
+  </si>
+  <si>
+    <t>Qn14</t>
+  </si>
+  <si>
+    <t>Qn6</t>
+  </si>
+  <si>
+    <t>Qn15</t>
+  </si>
+  <si>
+    <t>Qn16</t>
+  </si>
+  <si>
+    <t>Qn17</t>
+  </si>
+  <si>
+    <t>Qn19</t>
+  </si>
+  <si>
+    <t>Qn20</t>
+  </si>
+  <si>
+    <t>Qn24</t>
+  </si>
+  <si>
+    <t>Qn25</t>
+  </si>
+  <si>
+    <t>Qn27</t>
+  </si>
+  <si>
+    <t>Qn28</t>
+  </si>
+  <si>
+    <t>Qn29</t>
+  </si>
+  <si>
+    <t>Qn74</t>
+  </si>
+  <si>
+    <t>Qn76</t>
+  </si>
+  <si>
+    <t>Qn77</t>
+  </si>
+  <si>
+    <t>Qn78</t>
+  </si>
+  <si>
+    <t>Qn80</t>
+  </si>
+  <si>
+    <t>Qn81</t>
+  </si>
+  <si>
+    <t>Qn4a</t>
+  </si>
+  <si>
+    <t>Qn4b</t>
+  </si>
+  <si>
+    <t>Qn4c</t>
+  </si>
+  <si>
+    <t>Qn4d</t>
+  </si>
+  <si>
+    <t>Qn4e</t>
+  </si>
+  <si>
+    <t>Qn5a</t>
+  </si>
+  <si>
+    <t>Qn5b</t>
+  </si>
+  <si>
+    <t>Qn5c</t>
+  </si>
+  <si>
+    <t>Qn5d</t>
+  </si>
+  <si>
+    <t>Qn5e</t>
+  </si>
+  <si>
+    <t>Qn18</t>
+  </si>
+  <si>
+    <t>Qn22</t>
+  </si>
+  <si>
+    <t>Qn23</t>
+  </si>
+  <si>
+    <t>Qn26</t>
+  </si>
+  <si>
+    <t>Qn30</t>
+  </si>
+  <si>
+    <t>Qn73</t>
+  </si>
+  <si>
+    <t>Qn75</t>
   </si>
 </sst>
 </file>
@@ -712,15 +844,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A998DB2-5187-45E8-AD8C-B2FFA1335107}">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="226.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:40" ht="289" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,34 +866,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
@@ -800,16 +932,16 @@
         <v>15</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>16</v>
@@ -817,8 +949,32 @@
       <c r="AF1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>2020</v>
       </c>
@@ -832,34 +988,34 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -901,13 +1057,13 @@
         <v>33</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>35</v>
@@ -915,397 +1071,517 @@
       <c r="AF2" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AG2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>2018</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>59</v>
+        <v>119</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>59</v>
+        <v>119</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>2016</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>99</v>
+        <v>140</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>